<commit_message>
modifiche float e outstanding da finiviz
</commit_message>
<xml_diff>
--- a/output/dati_azioni_completo_2025-09-29.xlsx
+++ b/output/dati_azioni_completo_2025-09-29.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ6"/>
+  <dimension ref="A1:AQ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,7 +679,7 @@
         <v>45929</v>
       </c>
       <c r="H2" t="n">
-        <v>8.41</v>
+        <v>8.25</v>
       </c>
       <c r="I2" t="n">
         <v>5.52</v>
@@ -700,13 +700,13 @@
         <v>8.49</v>
       </c>
       <c r="O2" t="n">
-        <v>52.36</v>
+        <v>49.46</v>
       </c>
       <c r="P2" t="n">
         <v>7.65</v>
       </c>
       <c r="Q2" t="n">
-        <v>-9.01</v>
+        <v>-7.25</v>
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
@@ -767,10 +767,10 @@
         </is>
       </c>
       <c r="AJ2" t="n">
-        <v>8.550000000000001</v>
+        <v>8.33</v>
       </c>
       <c r="AK2" t="n">
-        <v>8.19</v>
+        <v>8.220000000000001</v>
       </c>
       <c r="AL2" t="n">
         <v>8514909</v>
@@ -781,10 +781,10 @@
         </is>
       </c>
       <c r="AN2" t="n">
-        <v>8.550000000000001</v>
+        <v>8.33</v>
       </c>
       <c r="AO2" t="n">
-        <v>8.19</v>
+        <v>8.220000000000001</v>
       </c>
       <c r="AP2" t="n">
         <v>8514909</v>
@@ -808,7 +808,7 @@
         <v>5496900</v>
       </c>
       <c r="D3" t="n">
-        <v>4644079</v>
+        <v>3010000</v>
       </c>
       <c r="E3" t="n">
         <v>0.76403</v>
@@ -820,7 +820,7 @@
         <v>45929</v>
       </c>
       <c r="H3" t="n">
-        <v>11.21</v>
+        <v>10.72</v>
       </c>
       <c r="I3" t="n">
         <v>6.85</v>
@@ -841,13 +841,13 @@
         <v>11.16</v>
       </c>
       <c r="O3" t="n">
-        <v>63.65</v>
+        <v>56.5</v>
       </c>
       <c r="P3" t="n">
-        <v>11.56</v>
+        <v>11.55</v>
       </c>
       <c r="Q3" t="n">
-        <v>3.08</v>
+        <v>7.79</v>
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
@@ -908,10 +908,10 @@
         </is>
       </c>
       <c r="AJ3" t="n">
-        <v>11.21</v>
+        <v>10.9</v>
       </c>
       <c r="AK3" t="n">
-        <v>10.65</v>
+        <v>10.69</v>
       </c>
       <c r="AL3" t="n">
         <v>3784261</v>
@@ -922,10 +922,10 @@
         </is>
       </c>
       <c r="AN3" t="n">
-        <v>11.21</v>
+        <v>10.9</v>
       </c>
       <c r="AO3" t="n">
-        <v>10.65</v>
+        <v>10.69</v>
       </c>
       <c r="AP3" t="n">
         <v>3784261</v>
@@ -949,7 +949,7 @@
         <v>17450476</v>
       </c>
       <c r="D4" t="n">
-        <v>7050569</v>
+        <v>2930000</v>
       </c>
       <c r="E4" t="n">
         <v>0.77935</v>
@@ -961,7 +961,7 @@
         <v>45929</v>
       </c>
       <c r="H4" t="n">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="I4" t="n">
         <v>0.95</v>
@@ -982,18 +982,18 @@
         <v>3.79</v>
       </c>
       <c r="O4" t="n">
-        <v>297.91</v>
+        <v>292.67</v>
       </c>
       <c r="P4" t="n">
         <v>1.64</v>
       </c>
       <c r="Q4" t="n">
-        <v>-56.89</v>
+        <v>-56.31</v>
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="n">
-        <v>3.96</v>
+        <v>3.93</v>
       </c>
       <c r="U4" t="n">
         <v>2.42</v>
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="X4" t="n">
-        <v>3.96</v>
+        <v>3.93</v>
       </c>
       <c r="Y4" t="n">
         <v>2.03</v>
@@ -1021,7 +1021,7 @@
         </is>
       </c>
       <c r="AB4" t="n">
-        <v>3.96</v>
+        <v>3.93</v>
       </c>
       <c r="AC4" t="n">
         <v>1.91</v>
@@ -1035,7 +1035,7 @@
         </is>
       </c>
       <c r="AF4" t="n">
-        <v>3.96</v>
+        <v>3.93</v>
       </c>
       <c r="AG4" t="n">
         <v>1.31</v>
@@ -1049,7 +1049,7 @@
         </is>
       </c>
       <c r="AJ4" t="n">
-        <v>3.96</v>
+        <v>3.75</v>
       </c>
       <c r="AK4" t="n">
         <v>3.41</v>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="AN4" t="n">
-        <v>3.96</v>
+        <v>3.75</v>
       </c>
       <c r="AO4" t="n">
         <v>3.41</v>
@@ -1102,7 +1102,7 @@
         <v>45929</v>
       </c>
       <c r="H5" t="n">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="I5" t="n">
         <v>0.77</v>
@@ -1123,18 +1123,18 @@
         <v>2.14</v>
       </c>
       <c r="O5" t="n">
-        <v>175.48</v>
+        <v>158.06</v>
       </c>
       <c r="P5" t="n">
         <v>1.49</v>
       </c>
       <c r="Q5" t="n">
-        <v>-30.27</v>
+        <v>-25.56</v>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="n">
-        <v>2.13</v>
+        <v>2.03</v>
       </c>
       <c r="U5" t="n">
         <v>1.37</v>
@@ -1148,7 +1148,7 @@
         </is>
       </c>
       <c r="X5" t="n">
-        <v>2.13</v>
+        <v>2.03</v>
       </c>
       <c r="Y5" t="n">
         <v>1.37</v>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="AB5" t="n">
-        <v>2.13</v>
+        <v>2.03</v>
       </c>
       <c r="AC5" t="n">
         <v>1.28</v>
@@ -1176,7 +1176,7 @@
         </is>
       </c>
       <c r="AF5" t="n">
-        <v>2.13</v>
+        <v>2.03</v>
       </c>
       <c r="AG5" t="n">
         <v>1.28</v>
@@ -1190,10 +1190,10 @@
         </is>
       </c>
       <c r="AJ5" t="n">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="AK5" t="n">
-        <v>1.9</v>
+        <v>1.92</v>
       </c>
       <c r="AL5" t="n">
         <v>9319030</v>
@@ -1204,10 +1204,10 @@
         </is>
       </c>
       <c r="AN5" t="n">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="AO5" t="n">
-        <v>1.9</v>
+        <v>1.92</v>
       </c>
       <c r="AP5" t="n">
         <v>9319030</v>
@@ -1221,139 +1221,280 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ZURA</t>
+          <t>RDHL</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>194403984</v>
+        <v>7791872</v>
       </c>
       <c r="C6" t="n">
-        <v>65018058</v>
+        <v>3329860</v>
       </c>
       <c r="D6" t="n">
-        <v>37881471</v>
+        <v>3310000</v>
       </c>
       <c r="E6" t="n">
-        <v>0.27749002</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.51230997</v>
+        <v>0.0269</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>45929</v>
       </c>
       <c r="H6" t="n">
-        <v>3.59</v>
+        <v>2.5</v>
       </c>
       <c r="I6" t="n">
-        <v>2.41</v>
+        <v>1.84</v>
       </c>
       <c r="J6" t="n">
-        <v>3.74</v>
+        <v>2.79</v>
       </c>
       <c r="K6" t="n">
-        <v>2.76</v>
+        <v>2.01</v>
       </c>
       <c r="L6" t="n">
-        <v>2.99</v>
+        <v>2.34</v>
       </c>
       <c r="M6" t="n">
-        <v>25401700</v>
+        <v>55704600</v>
       </c>
       <c r="N6" t="n">
-        <v>3.59</v>
+        <v>2.58</v>
       </c>
       <c r="O6" t="n">
-        <v>48.76</v>
+        <v>35.87</v>
       </c>
       <c r="P6" t="n">
-        <v>3.24</v>
+        <v>2.34</v>
       </c>
       <c r="Q6" t="n">
-        <v>-9.550000000000001</v>
+        <v>-6.29</v>
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="U6" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="V6" t="n">
+        <v>22893516</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="X6" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>50923227</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="AB6" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>51481031</v>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="AF6" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>79789126</v>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="AJ6" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>17197546</v>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AN6" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>17197546</v>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ZURA</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>194403984</v>
+      </c>
+      <c r="C7" t="n">
+        <v>65018058</v>
+      </c>
+      <c r="D7" t="n">
+        <v>37881471</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.27749002</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.51230997</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="J7" t="n">
         <v>3.74</v>
       </c>
-      <c r="U6" t="n">
+      <c r="K7" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="M7" t="n">
+        <v>25401700</v>
+      </c>
+      <c r="N7" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="O7" t="n">
+        <v>45.23</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-7.35</v>
+      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="U7" t="n">
         <v>2.9</v>
       </c>
-      <c r="V6" t="n">
+      <c r="V7" t="n">
         <v>15805544</v>
       </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="X6" t="n">
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="X7" t="n">
         <v>3.74</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="Y7" t="n">
         <v>2.76</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="Z7" t="n">
         <v>21938495</v>
       </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AB6" t="n">
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="AB7" t="n">
         <v>3.74</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AC7" t="n">
         <v>2.76</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="AD7" t="n">
         <v>24042193</v>
       </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AF6" t="n">
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="AF7" t="n">
         <v>3.74</v>
       </c>
-      <c r="AG6" t="n">
+      <c r="AG7" t="n">
         <v>2.76</v>
       </c>
-      <c r="AH6" t="n">
+      <c r="AH7" t="n">
         <v>48961363</v>
       </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="AJ6" t="n">
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="AJ7" t="n">
         <v>3.72</v>
       </c>
-      <c r="AK6" t="n">
+      <c r="AK7" t="n">
         <v>3.49</v>
       </c>
-      <c r="AL6" t="n">
+      <c r="AL7" t="n">
         <v>3847520</v>
       </c>
-      <c r="AM6" t="inlineStr">
+      <c r="AM7" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="AN6" t="n">
+      <c r="AN7" t="n">
         <v>3.72</v>
       </c>
-      <c r="AO6" t="n">
+      <c r="AO7" t="n">
         <v>3.49</v>
       </c>
-      <c r="AP6" t="n">
+      <c r="AP7" t="n">
         <v>3847520</v>
       </c>
-      <c r="AQ6" t="inlineStr">
+      <c r="AQ7" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>

</xml_diff>